<commit_message>
Hotfix Delete JsonXAI argument
</commit_message>
<xml_diff>
--- a/R+D/research/Evaluation-2.xlsx
+++ b/R+D/research/Evaluation-2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\osins\Desktop\R&amp;D Project\lm-evaluation-harness\R+D\research\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{975ED2EB-682B-4903-A76B-A553DAD8D7D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DEED9A6-6244-490B-81E2-12A5B765CC9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="5" xr2:uid="{76F17BED-C1F5-429D-A3BE-DE652BCF7AB9}"/>
+    <workbookView xWindow="1605" yWindow="2655" windowWidth="21600" windowHeight="11175" activeTab="5" xr2:uid="{76F17BED-C1F5-429D-A3BE-DE652BCF7AB9}"/>
   </bookViews>
   <sheets>
     <sheet name="POC" sheetId="1" r:id="rId1"/>
@@ -79,7 +79,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="684" uniqueCount="337">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="707" uniqueCount="354">
   <si>
     <t>MODEL</t>
   </si>
@@ -1090,6 +1090,57 @@
   </si>
   <si>
     <t>curl 34.207.226.68:8080/factors/10</t>
+  </si>
+  <si>
+    <t>winograde</t>
+  </si>
+  <si>
+    <t>head_qa_en</t>
+  </si>
+  <si>
+    <t>✅</t>
+  </si>
+  <si>
+    <t>arc_challenge_mt_pl</t>
+  </si>
+  <si>
+    <t>ethics_cm</t>
+  </si>
+  <si>
+    <t>mmlu_pro</t>
+  </si>
+  <si>
+    <t>truthfulqa_gen</t>
+  </si>
+  <si>
+    <t>truthfulqa_mc1</t>
+  </si>
+  <si>
+    <t>webqs</t>
+  </si>
+  <si>
+    <t>nq_open</t>
+  </si>
+  <si>
+    <t>sudo yum install git -y</t>
+  </si>
+  <si>
+    <t>git clone https://git.wmi.amu.edu.pl/s444820/cloud-aws-webservice.git</t>
+  </si>
+  <si>
+    <t>cd cloud-aws-webservice/</t>
+  </si>
+  <si>
+    <t>sudo yum install iptables-services -y</t>
+  </si>
+  <si>
+    <t>sudo iptables -t nat -A PREROUTING -p tcp --dport 80 -j REDIRECT --to-port 8080</t>
+  </si>
+  <si>
+    <t>./webservice</t>
+  </si>
+  <si>
+    <t>sudo chmod +x ./webservice</t>
   </si>
 </sst>
 </file>
@@ -38007,7 +38058,7 @@
   <dimension ref="A1:AB6"/>
   <sheetViews>
     <sheetView topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="S5" sqref="S5"/>
+      <selection activeCell="N1" sqref="N1:P1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -39163,10 +39214,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{533557A5-8F9C-4270-B197-C402D9A86FC7}">
-  <dimension ref="C5:H20"/>
+  <dimension ref="C5:J31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P27" sqref="P27"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="J25" sqref="J25:J31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -39180,6 +39231,9 @@
       <c r="C6" t="s">
         <v>321</v>
       </c>
+      <c r="D6" t="s">
+        <v>339</v>
+      </c>
       <c r="E6" s="44" t="s">
         <v>331</v>
       </c>
@@ -39191,6 +39245,9 @@
       <c r="C7" t="s">
         <v>188</v>
       </c>
+      <c r="D7" t="s">
+        <v>339</v>
+      </c>
       <c r="E7" t="s">
         <v>333</v>
       </c>
@@ -39217,11 +39274,17 @@
       <c r="C12" t="s">
         <v>325</v>
       </c>
+      <c r="D12" t="s">
+        <v>339</v>
+      </c>
     </row>
     <row r="13" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C13" t="s">
         <v>326</v>
       </c>
+      <c r="D13" t="s">
+        <v>339</v>
+      </c>
     </row>
     <row r="14" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C14" t="s">
@@ -39232,17 +39295,105 @@
       <c r="C15" t="s">
         <v>328</v>
       </c>
+      <c r="D15" t="s">
+        <v>339</v>
+      </c>
       <c r="H15" t="s">
         <v>335</v>
       </c>
     </row>
-    <row r="20" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C16" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="17" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C17" t="s">
+        <v>338</v>
+      </c>
+      <c r="D17" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="18" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C18" t="s">
+        <v>340</v>
+      </c>
+      <c r="D18" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="19" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C19" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="20" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C20" t="s">
+        <v>342</v>
+      </c>
       <c r="H20" t="s">
         <v>336</v>
+      </c>
+    </row>
+    <row r="21" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C21" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="22" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C22" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="23" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C23" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="24" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C24" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="25" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="J25" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="26" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="J26" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="27" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="J27" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="28" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="J28" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="29" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="J29" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="30" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="J30" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="31" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="J31" t="s">
+        <v>352</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>